<commit_message>
1.2 changes for pass through charging and mounting
</commit_message>
<xml_diff>
--- a/PCB/V1.1BOM:POS/PCB_BOM.xlsx
+++ b/PCB/V1.1BOM:POS/PCB_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Comment</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>PQFN80P500X300X100-14N</t>
+  </si>
+  <si>
+    <t>D39</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -138,13 +141,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -157,13 +197,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -383,9 +429,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -417,10 +466,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -659,9 +708,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -965,10 +1017,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1210,7 +1262,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1234,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1247,80 +1299,93 @@
         <v>5</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="14.7" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="A3" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="5">
+      <c r="C3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" t="s" s="5">
+      <c r="A4" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="5">
+      <c r="B4" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="5">
+      <c r="C4" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" t="s" s="5">
+      <c r="A5" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="5">
+      <c r="B5" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="C5" t="s" s="5">
+      <c r="C5" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" t="s" s="5">
+      <c r="A6" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="B6" t="s" s="5">
+      <c r="B6" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C6" t="s" s="5">
+      <c r="C6" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
+      <c r="A7" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>

</xml_diff>